<commit_message>
Ajutes fase 2 con seguridad y funcionalidad completa
</commit_message>
<xml_diff>
--- a/Homecenter/reportes/reporte.xlsx
+++ b/Homecenter/reportes/reporte.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="reporte" sheetId="1" r:id="R90b89f8dccef496f"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="reporte" sheetId="1" r:id="R51769b2ac93e4af8"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -18,19 +18,28 @@
         <x:v>Asesor</x:v>
       </x:c>
       <x:c t="str">
-        <x:v>Cédula</x:v>
+        <x:v>Cédula Asesor</x:v>
       </x:c>
       <x:c t="str">
-        <x:v>Código</x:v>
+        <x:v>Código Asesor</x:v>
       </x:c>
       <x:c t="str">
         <x:v>Tienda</x:v>
       </x:c>
       <x:c t="str">
-        <x:v>SKU</x:v>
+        <x:v>SKU Electrodoméstico</x:v>
       </x:c>
       <x:c t="str">
         <x:v>Fecha</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>Cédula cliente</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>SKU Garantía</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>Valor comisión</x:v>
       </x:c>
     </x:row>
     <x:row r="2">
@@ -50,13 +59,54 @@
         <x:v>112</x:v>
       </x:c>
       <x:c t="str">
+        <x:v>455675</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>2018-03-12 16.40.42</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>41669007</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>555666</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>1,35</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3">
+      <x:c t="str">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>Leandro Baena Torres</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>79726745</x:v>
+      </x:c>
+      <x:c t="str">
         <x:v>255657</x:v>
       </x:c>
       <x:c t="str">
-        <x:v>2018-03-09 10.59.05</x:v>
+        <x:v>112</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>567890</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>2018-03-12 16.58.16</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>4567890</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>555666</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>1,35</x:v>
       </x:c>
     </x:row>
-    <x:row r="3">
+    <x:row r="4">
       <x:c t="str">
         <x:v>3</x:v>
       </x:c>
@@ -73,33 +123,19 @@
         <x:v>112</x:v>
       </x:c>
       <x:c t="str">
-        <x:v>256566</x:v>
+        <x:v>345345</x:v>
       </x:c>
       <x:c t="str">
-        <x:v>2018-03-09 11.01.48</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="4">
-      <x:c t="str">
-        <x:v>4</x:v>
+        <x:v>2018-03-12 18.08.33</x:v>
       </x:c>
       <x:c t="str">
-        <x:v>David Santiago Baena Barreto</x:v>
+        <x:v>56767567</x:v>
       </x:c>
       <x:c t="str">
-        <x:v>1007105321</x:v>
+        <x:v>555666</x:v>
       </x:c>
       <x:c t="str">
-        <x:v>256566</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>120</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>123456</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>2018-03-09 11.04.39</x:v>
+        <x:v>1,35</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>